<commit_message>
updated spreadsheet for ihocl
</commit_message>
<xml_diff>
--- a/hocl_coords.xlsx
+++ b/hocl_coords.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coire/McCoy/hocl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC765FA4-A8C0-5A42-8FF3-C6D208ACF6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB681A-4CD2-084A-B53C-A42586E97655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="30480" windowHeight="21900" activeTab="1"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="17360" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clhocl" sheetId="1" r:id="rId1"/>
     <sheet name="clhocl_2" sheetId="2" r:id="rId2"/>
+    <sheet name="brhocl" sheetId="3" r:id="rId3"/>
+    <sheet name="ihocl" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="29">
   <si>
     <t>r1</t>
   </si>
@@ -114,11 +116,17 @@
   <si>
     <t>rad</t>
   </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -384,16 +392,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -405,25 +407,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="14"/>
-    <cellStyle name="Text" xfId="15"/>
-    <cellStyle name="Warning" xfId="16"/>
+    <cellStyle name="Status" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Text" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Warning" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -831,11 +842,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -851,11 +862,11 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -872,11 +883,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -893,11 +904,11 @@
         <f>B4*SIN(C6)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="1">
@@ -976,11 +987,11 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
@@ -996,11 +1007,11 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
@@ -1017,11 +1028,11 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
@@ -1038,11 +1049,11 @@
         <f>B18*SIN(C20)</f>
         <v>0.26617623527860501</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="1">
@@ -1127,11 +1138,11 @@
       <c r="D35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
@@ -1147,11 +1158,11 @@
       <c r="D36" s="2">
         <v>0</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
@@ -1168,11 +1179,11 @@
       <c r="D37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
@@ -1189,11 +1200,11 @@
         <f>B31*SIN(C33)</f>
         <v>0.49928084499999992</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8">
       <c r="F39" s="2"/>
@@ -1298,9 +1309,9 @@
       <c r="D47" s="2">
         <v>0</v>
       </c>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
@@ -1316,9 +1327,9 @@
       <c r="D48" s="2">
         <v>0</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
@@ -1335,9 +1346,9 @@
       <c r="D49" s="2">
         <v>0</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
@@ -1354,11 +1365,11 @@
         <f>B43*SIN(C45)</f>
         <v>0.69469717031380851</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
     </row>
     <row r="51" spans="1:8">
       <c r="F51" s="2"/>
@@ -1463,9 +1474,9 @@
       <c r="D59" s="2">
         <v>0</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
@@ -1481,9 +1492,9 @@
       <c r="D60" s="2">
         <v>0</v>
       </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
@@ -1500,9 +1511,9 @@
       <c r="D61" s="2">
         <v>0</v>
       </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
@@ -1519,11 +1530,11 @@
         <f>B55*SIN(C57)</f>
         <v>0.84307381666800862</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
     </row>
     <row r="63" spans="1:8">
       <c r="F63" s="2"/>
@@ -1628,9 +1639,9 @@
       <c r="D71" s="2">
         <v>0</v>
       </c>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
@@ -1646,9 +1657,9 @@
       <c r="D72" s="2">
         <v>0</v>
       </c>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
@@ -1665,9 +1676,9 @@
       <c r="D73" s="2">
         <v>0</v>
       </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
@@ -1684,19 +1695,14 @@
         <f>B67*SIN(C69)</f>
         <v>0.93693120575398581</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F74" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="F48:H48"/>
@@ -1704,11 +1710,11 @@
     <mergeCell ref="F50:H50"/>
     <mergeCell ref="F59:H59"/>
     <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
@@ -1716,6 +1722,11 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <headerFooter>
@@ -1726,10 +1737,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1778,7 +1789,7 @@
       <c r="G4">
         <v>5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>1.0276700000000001</v>
       </c>
     </row>
@@ -1796,7 +1807,7 @@
       <c r="G5">
         <v>10</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>1.02355</v>
       </c>
     </row>
@@ -1814,7 +1825,7 @@
       <c r="G6">
         <v>15</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>1.0180899999999999</v>
       </c>
     </row>
@@ -1822,7 +1833,7 @@
       <c r="G7">
         <v>20</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>1.01156</v>
       </c>
     </row>
@@ -1830,7 +1841,7 @@
       <c r="G8">
         <v>25</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>1.0052300000000001</v>
       </c>
     </row>
@@ -1847,70 +1858,70 @@
       <c r="G9">
         <v>30</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>0.99856999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
         <v>0</v>
       </c>
       <c r="G10">
         <v>35</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>0.99243000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <f>C3</f>
         <v>2.9046759999999998</v>
       </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
         <v>0</v>
       </c>
       <c r="G11">
         <v>40</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>0.98668</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <f>C2*COS(D5)</f>
         <v>-0.39368663955435501</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <f>C2*SIN(D5)</f>
         <v>1.6360486016122504</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>0</v>
       </c>
       <c r="G12">
         <v>45</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>0.98224</v>
       </c>
     </row>
@@ -1936,7 +1947,7 @@
       <c r="G13">
         <v>50</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <v>0.97858999999999996</v>
       </c>
     </row>
@@ -1968,7 +1979,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B14:B31" si="2">A15*2*PI()/360</f>
+        <f t="shared" ref="B15:B31" si="2">A15*2*PI()/360</f>
         <v>0.17453292519943295</v>
       </c>
       <c r="C15">
@@ -2335,4 +2346,1234 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A425715-90E8-2848-917D-6DB65931FF06}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.68432553</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.0738174699999998</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.0177400000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0284260000000001</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.01715</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>103.42034752000001</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5*2*PI()/360</f>
+        <v>1.8050255777807522</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.01433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f>C6*(2*PI())/360</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.0103800000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18">
+      <c r="G7" s="3">
+        <v>20</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.00553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18">
+      <c r="G8" s="3">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.0002899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18">
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.99504000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>35</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.99007999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18">
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9">
+        <f>C3</f>
+        <v>3.0738174699999998</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>40</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.98560999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18">
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12">
+        <f>C2*COS(D5)</f>
+        <v>-0.39092075804302223</v>
+      </c>
+      <c r="D12" s="12">
+        <f>C2*SIN(D5)</f>
+        <v>1.6383325217857483</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.98173999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18">
+      <c r="A13" s="3">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <f>A13*2*PI()/360</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <f>H3*COS(B13)</f>
+        <v>1.0177400000000001</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <f>H3*SIN(B13)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>50</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.97850000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <f>A14*2*PI()/360</f>
+        <v>8.7266462599716474E-2</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" ref="C14:C31" si="0">H4*COS(B14)</f>
+        <v>1.013279437164019</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ref="E14:E31" si="1">H4*SIN(B14)</f>
+        <v>8.8650463735780505E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:B31" si="2">A15*2*PI()/360</f>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99892004811287294</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.17613655605289744</v>
+      </c>
+      <c r="G15" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="2"/>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="C16" s="3">
+        <f>H6*COS(B16)</f>
+        <v>0.97595213636594891</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150558679068492</v>
+      </c>
+      <c r="G16" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.94488912097885458</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.34391151471825965</v>
+      </c>
+      <c r="G17" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.43633231299858238</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.90657061629489044</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <f>H8*SIN(B18)</f>
+        <v>0.42274082103660421</v>
+      </c>
+      <c r="G18" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.86172991778166796</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49751999999999996</v>
+      </c>
+      <c r="G19" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6108652381980153</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.81102605600964495</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.56788655810244359</v>
+      </c>
+      <c r="G20" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="3">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.69813170079773179</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75502106358249588</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.63353789598314991</v>
+      </c>
+      <c r="G21" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>0.69419501136208117</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.69419500999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3">
+        <v>50</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87266462599716477</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.62896767607827875</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.74957448759192002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95993108859688125</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="3">
+        <v>60</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3">
+        <v>65</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1344640137963142</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="3">
+        <v>70</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2217304763960306</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3">
+        <v>75</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="3">
+        <v>80</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3962634015954636</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="3">
+        <v>85</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4835298641951802</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="3">
+        <v>90</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52B69D2-8EF1-DD43-9B91-7BB47DD94404}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.6865217400000001</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18">
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.3122984099999999</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.0080499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18">
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1.0080509099999999</v>
+      </c>
+      <c r="G4" s="14">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.00762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18">
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>103.24536913999999</v>
+      </c>
+      <c r="D5" s="14">
+        <f>C5*2*PI()/360</f>
+        <v>1.8019716289299461</v>
+      </c>
+      <c r="G5" s="14">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.0057400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18">
+      <c r="B6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <f>C6*(2*PI())/360</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.00301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18">
+      <c r="G7" s="14">
+        <v>20</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.99958000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18">
+      <c r="G8" s="14">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.99573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18">
+      <c r="C9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="14">
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.99175000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>35</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.98787999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18">
+      <c r="B11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9">
+        <f>C3</f>
+        <v>3.3122984099999999</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>40</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.98429999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18">
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12">
+        <f>C2*COS(D5)</f>
+        <v>-0.38641875852655388</v>
+      </c>
+      <c r="D12" s="12">
+        <f>C2*SIN(D5)</f>
+        <v>1.6416565178353921</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>45</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.98111999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18">
+      <c r="A13" s="14">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14">
+        <f>A13*2*PI()/360</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="14">
+        <f>H3*COS(B13)</f>
+        <v>1.0080499999999999</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14">
+        <f>H3*SIN(B13)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>50</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.97838000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="14">
+        <f>A14*2*PI()/360</f>
+        <v>8.7266462599716474E-2</v>
+      </c>
+      <c r="C14" s="14">
+        <f>H4*COS(B14)</f>
+        <v>1.0037857016912046</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" ref="E14:E31" si="0">H4*SIN(B14)</f>
+        <v>8.7819869507395315E-2</v>
+      </c>
+      <c r="G14" s="14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="14">
+        <v>10</v>
+      </c>
+      <c r="B15" s="14">
+        <f t="shared" ref="B15:B31" si="1">A15*2*PI()/360</f>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="C15" s="14">
+        <f>H5*COS(B15)</f>
+        <v>0.99046054951449813</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="0"/>
+        <v>0.17464491820673853</v>
+      </c>
+      <c r="G15" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <f t="shared" si="1"/>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="C16" s="14">
+        <f>H6*COS(B16)</f>
+        <v>0.96883326302619832</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14">
+        <f>H6*SIN(B16)</f>
+        <v>0.2595980904282793</v>
+      </c>
+      <c r="G16" s="14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14">
+        <f t="shared" si="1"/>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="C17" s="14">
+        <f t="shared" ref="C14:C31" si="2">H7*COS(B17)</f>
+        <v>0.93929794988517834</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="0"/>
+        <v>0.34187649486547195</v>
+      </c>
+      <c r="G17" s="14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="14">
+        <v>25</v>
+      </c>
+      <c r="B18" s="14">
+        <f t="shared" si="1"/>
+        <v>0.43633231299858238</v>
+      </c>
+      <c r="C18" s="14">
+        <f t="shared" si="2"/>
+        <v>0.90243785278600341</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <f>H8*SIN(B18)</f>
+        <v>0.42081368176306666</v>
+      </c>
+      <c r="G18" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="14">
+        <v>30</v>
+      </c>
+      <c r="B19" s="14">
+        <f t="shared" si="1"/>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="C19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.85888069420321711</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="0"/>
+        <v>0.49587499999999995</v>
+      </c>
+      <c r="G19" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="14">
+        <v>35</v>
+      </c>
+      <c r="B20" s="14">
+        <f t="shared" si="1"/>
+        <v>0.6108652381980153</v>
+      </c>
+      <c r="C20" s="14">
+        <f t="shared" si="2"/>
+        <v>0.80922392151220923</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="0"/>
+        <v>0.56662468994247139</v>
+      </c>
+      <c r="G20" s="14">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="14">
+        <v>40</v>
+      </c>
+      <c r="B21" s="14">
+        <f t="shared" si="1"/>
+        <v>0.69813170079773179</v>
+      </c>
+      <c r="C21" s="14">
+        <f t="shared" si="2"/>
+        <v>0.75401754536201004</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="0"/>
+        <v>0.63269584421446057</v>
+      </c>
+      <c r="G21" s="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="14">
+        <v>45</v>
+      </c>
+      <c r="B22" s="14">
+        <f t="shared" si="1"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C22" s="14">
+        <f t="shared" si="2"/>
+        <v>0.69375660515774551</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.69419500999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="14">
+        <v>50</v>
+      </c>
+      <c r="B23" s="14">
+        <f t="shared" si="1"/>
+        <v>0.87266462599716477</v>
+      </c>
+      <c r="C23" s="14">
+        <f t="shared" si="2"/>
+        <v>0.62889054156511637</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="0"/>
+        <v>0.74948256225874577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="14">
+        <v>55</v>
+      </c>
+      <c r="B24" s="14">
+        <f t="shared" si="1"/>
+        <v>0.95993108859688125</v>
+      </c>
+      <c r="C24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0</v>
+      </c>
+      <c r="E24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="14">
+        <v>60</v>
+      </c>
+      <c r="B25" s="14">
+        <f t="shared" si="1"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="C25" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="14">
+        <v>65</v>
+      </c>
+      <c r="B26" s="14">
+        <f t="shared" si="1"/>
+        <v>1.1344640137963142</v>
+      </c>
+      <c r="C26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="14">
+        <v>0</v>
+      </c>
+      <c r="E26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="14">
+        <v>70</v>
+      </c>
+      <c r="B27" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2217304763960306</v>
+      </c>
+      <c r="C27" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0</v>
+      </c>
+      <c r="E27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="14">
+        <v>75</v>
+      </c>
+      <c r="B28" s="14">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="C28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="14">
+        <v>80</v>
+      </c>
+      <c r="B29" s="14">
+        <f t="shared" si="1"/>
+        <v>1.3962634015954636</v>
+      </c>
+      <c r="C29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0</v>
+      </c>
+      <c r="E29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="14">
+        <v>85</v>
+      </c>
+      <c r="B30" s="14">
+        <f t="shared" si="1"/>
+        <v>1.4835298641951802</v>
+      </c>
+      <c r="C30" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0</v>
+      </c>
+      <c r="E30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="14">
+        <v>90</v>
+      </c>
+      <c r="B31" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="14">
+        <v>0</v>
+      </c>
+      <c r="E31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>